<commit_message>
updates script and project metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_redd_project_metadata.xlsx
+++ b/data-raw/metadata/feather_redd_project_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\feather-redd\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C16C3F2-848D-42C8-AF70-EB143EC7DC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822146B0-4EE5-408C-8FB2-C01650227727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="19200" windowHeight="11170" tabRatio="834" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2660" yWindow="2660" windowWidth="19200" windowHeight="11170" tabRatio="834" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -1172,7 +1172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1234,7 +1234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
@@ -1292,6 +1292,7 @@
     <col min="3" max="3" width="22.6640625" customWidth="1"/>
     <col min="4" max="4" width="24.1640625" customWidth="1"/>
     <col min="5" max="5" width="23.83203125" customWidth="1"/>
+    <col min="6" max="7" width="16.25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="53.6640625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>